<commit_message>
update the folder name
</commit_message>
<xml_diff>
--- a/query.xlsx
+++ b/query.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Jira, Slack, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Jira, Slack, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -605,7 +605,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Jira, Slack, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Jira, Slack, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Jira, Slack, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Tableau, Power BI, Slack, Jira</t>
+          <t>Slack, Jira, Tableau, Power BI</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -891,7 +891,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1045,7 +1045,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>GitLab, Bitbucket, Docker, IntelliJ IDEA, Jenkins</t>
+          <t>Docker, IntelliJ IDEA, Bitbucket, GitLab, Jenkins</t>
         </is>
       </c>
     </row>

</xml_diff>